<commit_message>
alle animaties klaar opdracht 1
</commit_message>
<xml_diff>
--- a/uurrooster.xlsx
+++ b/uurrooster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sethv\Documents\GitHub\LUCA-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF495CD5-F163-44A0-AF66-E824C9A9340E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD1C294-A3CE-47D8-A7B4-8CF0108174CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="4" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="163">
   <si>
     <t>Week</t>
   </si>
@@ -556,9 +556,6 @@
     <t>oortjes voor crossmedia</t>
   </si>
   <si>
-    <t>weegschaal, credit card, pennenzak</t>
-  </si>
-  <si>
     <t>Curious drone geluid opnemen en monteren</t>
   </si>
   <si>
@@ -572,6 +569,15 @@
   </si>
   <si>
     <t>Filmpje moet klaar zijn video + ingediend</t>
+  </si>
+  <si>
+    <t>credit card, pennenzak</t>
+  </si>
+  <si>
+    <t>weegschaal</t>
+  </si>
+  <si>
+    <t>16.20 vertrekken naar SKI</t>
   </si>
 </sst>
 </file>
@@ -829,7 +835,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="241">
+  <dxfs count="239">
     <dxf>
       <fill>
         <patternFill>
@@ -2775,26 +2781,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color theme="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7995,22 +7987,22 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="B2:F3">
-    <cfRule type="expression" dxfId="240" priority="14">
+    <cfRule type="expression" dxfId="238" priority="14">
       <formula>B$3 &lt; TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:F3">
-    <cfRule type="expression" dxfId="239" priority="6">
+    <cfRule type="expression" dxfId="237" priority="6">
       <formula>B3 = TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:F25">
-    <cfRule type="expression" dxfId="238" priority="15">
+    <cfRule type="expression" dxfId="236" priority="15">
       <formula>$I$8 = TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:F36">
-    <cfRule type="expression" dxfId="237" priority="1">
+    <cfRule type="expression" dxfId="235" priority="1">
       <formula>NOT(ISBLANK(B28))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12758,30 +12750,30 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:D12">
-    <cfRule type="expression" dxfId="236" priority="3">
+    <cfRule type="expression" dxfId="234" priority="3">
       <formula>$I$8 = TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F3">
-    <cfRule type="expression" dxfId="235" priority="14">
+    <cfRule type="expression" dxfId="233" priority="14">
       <formula>B$3 = TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="234" priority="15">
+    <cfRule type="expression" dxfId="232" priority="15">
       <formula>B$3 &lt; TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:F36">
-    <cfRule type="expression" dxfId="233" priority="7">
+    <cfRule type="expression" dxfId="231" priority="7">
       <formula>NOT(ISBLANK(B28))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="232" priority="9">
+    <cfRule type="expression" dxfId="230" priority="9">
       <formula>NOT(ISBLANK(C13))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E6 B4:B13 F5:F6 E7:F25 D13 B14:D15 C16:D25">
-    <cfRule type="expression" dxfId="231" priority="12">
+    <cfRule type="expression" dxfId="229" priority="12">
       <formula>$I$8 = TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17665,22 +17657,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:F3">
-    <cfRule type="expression" dxfId="230" priority="10">
+    <cfRule type="expression" dxfId="228" priority="10">
       <formula>B$3 &lt; TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:F3">
-    <cfRule type="expression" dxfId="229" priority="9">
+    <cfRule type="expression" dxfId="227" priority="9">
       <formula>B3 = TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:F36">
-    <cfRule type="expression" dxfId="228" priority="1">
+    <cfRule type="expression" dxfId="226" priority="1">
       <formula>NOT(ISBLANK(B28))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:E6 F5:F6 B5:B14 C7:F8 C9:C13 E9:F13 C14:F14 B15:F15 C16:F25">
-    <cfRule type="expression" dxfId="227" priority="7">
+    <cfRule type="expression" dxfId="225" priority="7">
       <formula>$I$8 = TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18604,8 +18596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BECB010-7B12-49C5-982D-18AE879FB3BF}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -18954,7 +18946,7 @@
       <c r="E29" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="F29" s="19" t="s">
+      <c r="F29" s="23" t="s">
         <v>98</v>
       </c>
     </row>
@@ -18967,7 +18959,7 @@
       <c r="D30" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="23" t="s">
         <v>133</v>
       </c>
       <c r="F30" s="19" t="s">
@@ -18983,10 +18975,10 @@
       <c r="D31" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="E31" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="F31" s="19" t="s">
+      <c r="E31" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="F31" s="23" t="s">
         <v>146</v>
       </c>
     </row>
@@ -18999,11 +18991,11 @@
       <c r="D32" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="E32" s="23" t="s">
         <v>134</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.45">
@@ -19011,10 +19003,12 @@
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
-      <c r="E33" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="F33" s="19"/>
+      <c r="E33" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="11"/>
@@ -19022,7 +19016,9 @@
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
+      <c r="F34" s="19" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="11"/>
@@ -19041,59 +19037,49 @@
       <c r="F36" s="19"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B28 D28:F28 F31:F32 E31:E33">
-    <cfRule type="expression" dxfId="226" priority="15">
+  <conditionalFormatting sqref="B28 D28:F28">
+    <cfRule type="expression" dxfId="224" priority="15">
       <formula>NOT(ISBLANK(B28))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F3">
-    <cfRule type="expression" dxfId="225" priority="30">
+    <cfRule type="expression" dxfId="223" priority="30">
       <formula>B$3 &lt; TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:F3">
-    <cfRule type="expression" dxfId="224" priority="29">
+    <cfRule type="expression" dxfId="222" priority="29">
       <formula>B3 = TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:F29 B30:B33 B34:F36">
-    <cfRule type="expression" dxfId="223" priority="13">
+    <cfRule type="expression" dxfId="221" priority="13">
       <formula>NOT(ISBLANK(B29))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C33">
-    <cfRule type="expression" dxfId="222" priority="7">
+    <cfRule type="expression" dxfId="220" priority="7">
       <formula>NOT(ISBLANK(C28))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:D8 E6:E7 C9:C13 C14:D14">
-    <cfRule type="expression" dxfId="221" priority="24">
+    <cfRule type="expression" dxfId="219" priority="24">
       <formula>$I$8 = TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D25">
-    <cfRule type="expression" dxfId="220" priority="20">
+    <cfRule type="expression" dxfId="218" priority="20">
       <formula>$I$8 = TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31:D33">
-    <cfRule type="expression" dxfId="219" priority="2">
-      <formula>NOT(ISBLANK(D31))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30:F30">
-    <cfRule type="expression" dxfId="218" priority="12">
+  <conditionalFormatting sqref="D30:F33">
+    <cfRule type="expression" dxfId="217" priority="1">
       <formula>NOT(ISBLANK(D30))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F6 B5:B14 E7:F25 B15:D15 C16:C20 B16:B26 C21:D25">
-    <cfRule type="expression" dxfId="217" priority="25">
+    <cfRule type="expression" dxfId="216" priority="25">
       <formula>$I$8 = TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F33">
-    <cfRule type="expression" dxfId="216" priority="1">
-      <formula>NOT(ISBLANK(F33))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19105,8 +19091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C30AA62-9079-4511-A186-E2F20A9CFEA4}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView zoomScale="67" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -19421,7 +19407,7 @@
       <c r="D28" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="23" t="s">
         <v>137</v>
       </c>
       <c r="F28" s="16"/>
@@ -19429,14 +19415,14 @@
     <row r="29" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="11"/>
       <c r="B29" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C29" s="17"/>
       <c r="D29" s="19" t="s">
         <v>152</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F29" s="17"/>
     </row>
@@ -20618,7 +20604,7 @@
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
       <c r="E28" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F28" s="16"/>
     </row>

</xml_diff>

<commit_message>
backup just in case
</commit_message>
<xml_diff>
--- a/uurrooster.xlsx
+++ b/uurrooster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LUCA-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F247AEC7-3B53-472D-89AD-9A294A798D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3ABFF4-628D-4D89-8628-64D43C42E427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="4" r:id="rId1"/>
@@ -1232,7 +1232,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1321,6 +1321,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1331,7 +1337,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1340,8 +1346,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1459,9 +1466,13 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
+    <cellStyle name="20% - Accent3" xfId="8" builtinId="38"/>
     <cellStyle name="60% - Accent2" xfId="4" builtinId="36"/>
     <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
     <cellStyle name="60% - Accent6" xfId="6" builtinId="52"/>
@@ -5835,7 +5846,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7852,7 +7863,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8049,7 +8060,7 @@
         <v>323</v>
       </c>
       <c r="E17" s="34"/>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="67" t="s">
         <v>334</v>
       </c>
     </row>

</xml_diff>